<commit_message>
lab sharp and ultrasound with lcd just measuring distances
</commit_message>
<xml_diff>
--- a/LAB MICROS/lab1/matrix pinout.xlsx
+++ b/LAB MICROS/lab1/matrix pinout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unimilitareduco-my.sharepoint.com/personal/est_daniel_garciaa_unimilitar_edu_co/Documents/Documentos/UNIVERSIDADDDDDDDDDDDDDDDDDDDDDDDDDD/MECATRÓNICA/QUINTO SEMESTRE/MICROCONTROLERS/LAB MICROS/lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC275402-9B65-416A-A832-52A06F15D2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{BC275402-9B65-416A-A832-52A06F15D2E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE14FD52-CE5A-4687-9FDA-54CFC25AEB89}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ABAE068B-D61F-410F-8943-86A05DDC2B15}"/>
+    <workbookView xWindow="10395" yWindow="3255" windowWidth="21600" windowHeight="11295" xr2:uid="{ABAE068B-D61F-410F-8943-86A05DDC2B15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>A0</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
@@ -254,52 +251,28 @@
     <t>H7</t>
   </si>
   <si>
-    <t>b1</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
-    <t>f4</t>
-  </si>
-  <si>
-    <t>b6</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>d13</t>
-  </si>
-  <si>
-    <t>d12</t>
-  </si>
-  <si>
-    <t>d11</t>
-  </si>
-  <si>
-    <t>e2</t>
-  </si>
-  <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>b0</t>
-  </si>
-  <si>
-    <t>e0</t>
-  </si>
-  <si>
-    <t>e14</t>
-  </si>
-  <si>
-    <t>e15</t>
-  </si>
-  <si>
-    <t>b10</t>
-  </si>
-  <si>
-    <t>b11</t>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>C11</t>
+  </si>
+  <si>
+    <t>C12</t>
+  </si>
+  <si>
+    <t>mascara</t>
+  </si>
+  <si>
+    <t>cara</t>
+  </si>
+  <si>
+    <t>a00</t>
   </si>
 </sst>
 </file>
@@ -383,6 +356,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -702,41 +679,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFB51FE2-18B9-4561-BE0D-C86F69A180AC}">
-  <dimension ref="A3:K13"/>
+  <dimension ref="A3:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="4.140625" customWidth="1"/>
+    <col min="5" max="5" width="4" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="3.28515625" customWidth="1"/>
+    <col min="11" max="11" width="4.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="H3" t="s">
-        <v>76</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="J3" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D4" s="4">
         <v>13</v>
       </c>
@@ -762,7 +749,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1">
         <v>0</v>
@@ -789,9 +776,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B6" s="5">
         <v>9</v>
@@ -800,273 +787,695 @@
         <v>0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1</v>
+        <v>78</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="K6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B7" s="5">
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B8" s="5">
         <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B9" s="5">
         <v>12</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K9" s="2" t="s">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B12" s="5">
         <v>2</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="B13" s="5">
         <v>5</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>71</v>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>